<commit_message>
Atualizando o burndown e adicionando o 1.0 do mer
</commit_message>
<xml_diff>
--- a/Docs/Burndown/BurndownChart Sprint 3.xlsx
+++ b/Docs/Burndown/BurndownChart Sprint 3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\OneDrive\Documentos\GitHub\Fazenda-Urbana\Docs\Burndown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Luiz\Desktop\Fazenda-Urbana\Docs\Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D086F36-5D09-4BB4-832E-05F0EAA548F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E299726-39A3-455A-A132-92895E3377FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7BA74DF6-2A1D-4A46-8400-2B3B0F69CD68}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BA74DF6-2A1D-4A46-8400-2B3B0F69CD68}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="2" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Atual</t>
   </si>
@@ -62,41 +51,53 @@
     <t>Gráfico</t>
   </si>
   <si>
-    <t>18/04/2024</t>
-  </si>
-  <si>
-    <t>19/04/2024</t>
-  </si>
-  <si>
-    <t>20/04/2024</t>
-  </si>
-  <si>
-    <t>21/04/2024</t>
-  </si>
-  <si>
-    <t>23/04/2024</t>
-  </si>
-  <si>
-    <t>22/04/2024</t>
-  </si>
-  <si>
     <t>24/04/2024</t>
   </si>
   <si>
-    <t>Requisito do Usuário e requisito do sistema</t>
+    <t>25/04/2024</t>
   </si>
   <si>
-    <t>Elaborar os diagramas de classes de análise</t>
+    <t>26/04/2024</t>
   </si>
   <si>
-    <t>Explicar oque é ESG e seu relacionamento com os princípios da ODS</t>
+    <t>27/04/2024</t>
+  </si>
+  <si>
+    <t>28/04/2024</t>
+  </si>
+  <si>
+    <t>29/04/2024</t>
+  </si>
+  <si>
+    <t>30/04/2024</t>
+  </si>
+  <si>
+    <t>7)Gerar o script de criação de bancos e scripts de dados iniciais de testes (Roteiro de teste)</t>
+  </si>
+  <si>
+    <t>11) Elaborar o manual de uso do sistema para treinamento:</t>
+  </si>
+  <si>
+    <t>13) Elaborar protótipos de telas:</t>
+  </si>
+  <si>
+    <t>9) Requisito do Usuário e requisito do sistema:</t>
+  </si>
+  <si>
+    <t>2)Diagrama de implementação e Diagrama de sequência:</t>
+  </si>
+  <si>
+    <t>6)Elaborar o diagrama ER do banco de dados e o dicionário de dados:</t>
+  </si>
+  <si>
+    <t>4) Definir e justificar o ciclo de vida de desenvolvimento de software:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +137,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -304,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -372,6 +381,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,7 +490,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="pt-BR"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -514,25 +529,25 @@
                   <c:v>Start</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18/04/2024</c:v>
+                  <c:v>24/04/2024</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19/04/2024</c:v>
+                  <c:v>25/04/2024</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20/04/2024</c:v>
+                  <c:v>26/04/2024</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21/04/2024</c:v>
+                  <c:v>27/04/2024</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22/04/2024</c:v>
+                  <c:v>28/04/2024</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23/04/2024</c:v>
+                  <c:v>29/04/2024</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24/04/2024</c:v>
+                  <c:v>30/04/2024</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -544,22 +559,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -635,7 +650,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="pt-BR"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -674,25 +689,25 @@
                   <c:v>Start</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18/04/2024</c:v>
+                  <c:v>24/04/2024</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19/04/2024</c:v>
+                  <c:v>25/04/2024</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20/04/2024</c:v>
+                  <c:v>26/04/2024</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21/04/2024</c:v>
+                  <c:v>27/04/2024</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22/04/2024</c:v>
+                  <c:v>28/04/2024</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23/04/2024</c:v>
+                  <c:v>29/04/2024</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24/04/2024</c:v>
+                  <c:v>30/04/2024</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -704,28 +719,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -809,7 +824,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1266729296"/>
@@ -878,7 +893,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1862399680"/>
@@ -919,7 +934,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -959,7 +974,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1900,7 +1915,7 @@
   <dimension ref="B1:S58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1968,16 +1983,14 @@
       <c r="R4" s="19"/>
       <c r="S4" s="19"/>
     </row>
-    <row r="5" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" ht="57" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>14</v>
-      </c>
+      <c r="C5" s="12"/>
       <c r="D5" s="16" t="str">
         <f>IF(ISBLANK(C5),"Não Concluída","Concluída")</f>
-        <v>Concluída</v>
+        <v>Não Concluída</v>
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
@@ -1998,12 +2011,10 @@
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>13</v>
-      </c>
+      <c r="C6" s="13"/>
       <c r="D6" s="17" t="str">
         <f>IF(ISBLANK(C6),"Não Concluída","Concluída")</f>
-        <v>Concluída</v>
+        <v>Não Concluída</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
@@ -2020,16 +2031,14 @@
       <c r="R6" s="19"/>
       <c r="S6" s="19"/>
     </row>
-    <row r="7" spans="2:19" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="C7" s="12"/>
       <c r="D7" s="16" t="str">
         <f>IF(ISBLANK(C7),"Não Concluída","Concluída")</f>
-        <v>Concluída</v>
+        <v>Não Concluída</v>
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
@@ -2047,9 +2056,14 @@
       <c r="S7" s="19"/>
     </row>
     <row r="8" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="C8" s="13"/>
-      <c r="D8" s="17"/>
+      <c r="D8" s="16" t="str">
+        <f t="shared" ref="D8:D11" si="0">IF(ISBLANK(C8),"Não Concluída","Concluída")</f>
+        <v>Não Concluída</v>
+      </c>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
@@ -2066,9 +2080,14 @@
       <c r="S8" s="19"/>
     </row>
     <row r="9" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="C9" s="12"/>
-      <c r="D9" s="16"/>
+      <c r="D9" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>Não Concluída</v>
+      </c>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
@@ -2084,10 +2103,15 @@
       <c r="R9" s="19"/>
       <c r="S9" s="19"/>
     </row>
-    <row r="10" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="17"/>
+    <row r="10" spans="2:19" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>Não Concluída</v>
+      </c>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -2103,10 +2127,15 @@
       <c r="R10" s="19"/>
       <c r="S10" s="19"/>
     </row>
-    <row r="11" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
+    <row r="11" spans="2:19" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="C11" s="14"/>
-      <c r="D11" s="16"/>
+      <c r="D11" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>Não Concluída</v>
+      </c>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
@@ -2210,10 +2239,10 @@
         <v>11</v>
       </c>
       <c r="M20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N20" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>14</v>
@@ -2227,22 +2256,22 @@
         <v>1</v>
       </c>
       <c r="H21" s="1">
+        <v>7</v>
+      </c>
+      <c r="I21" s="1">
+        <v>6</v>
+      </c>
+      <c r="J21" s="1">
+        <v>5</v>
+      </c>
+      <c r="K21" s="1">
+        <v>4</v>
+      </c>
+      <c r="L21" s="1">
         <v>3</v>
       </c>
-      <c r="I21" s="1">
-        <v>3</v>
-      </c>
-      <c r="J21" s="1">
-        <v>3</v>
-      </c>
-      <c r="K21" s="1">
+      <c r="M21" s="1">
         <v>2</v>
-      </c>
-      <c r="L21" s="1">
-        <v>2</v>
-      </c>
-      <c r="M21" s="1">
-        <v>1</v>
       </c>
       <c r="N21" s="1">
         <v>1</v>
@@ -2259,35 +2288,35 @@
         <v>0</v>
       </c>
       <c r="H22" s="1">
-        <v>3</v>
-      </c>
-      <c r="I22" s="1">
-        <f>H22-COUNTIF($C$5:$C$10,I20)</f>
-        <v>3</v>
-      </c>
-      <c r="J22" s="1">
-        <f t="shared" ref="J22:O22" si="0">I22-COUNTIF($C$5:$C$10,J20)</f>
-        <v>3</v>
-      </c>
-      <c r="K22" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L22" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="M22" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="N22" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="O22" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="I22" s="23">
+        <f>H22-COUNTIF($C$5:$C$11,I20)</f>
+        <v>7</v>
+      </c>
+      <c r="J22" s="23">
+        <f t="shared" ref="J22:O22" si="1">I22-COUNTIF($C$5:$C$11,J20)</f>
+        <v>7</v>
+      </c>
+      <c r="K22" s="23">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="L22" s="23">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="M22" s="23">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="N22" s="23">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="O22" s="23">
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2476,16 +2505,19 @@
     <mergeCell ref="B2:S2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C58 C12 C14 C16 C18 C20 C22 C24 C26 C28 C30 C32 C34 C36 C38 C40 C42 C44 C46 C48 C50 C52 C54 C56 C8:C10" xr:uid="{7916BFD7-4F52-48BB-AC13-B3A91C73A66F}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C58 C12 C14 C16 C18 C20 C22 C24 C26 C28 C30 C32 C34 C36 C38 C40 C42 C44 C46 C48 C50 C52 C54 C56" xr:uid="{7916BFD7-4F52-48BB-AC13-B3A91C73A66F}">
       <formula1>$I$20:$K$20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C7" xr:uid="{70B2616D-06B6-4BFE-ABE8-20F72E5AA62A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C7 C11 C9 C8" xr:uid="{70B2616D-06B6-4BFE-ABE8-20F72E5AA62A}">
+      <formula1>$I$20:$O$20</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{F68F4EE4-6069-4FD0-9DAA-8C38F2DA31D0}">
       <formula1>$I$20:$O$20</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizando o Der, e 1.0 do cenario detalhado sobre o projeto
</commit_message>
<xml_diff>
--- a/Docs/Burndown/BurndownChart Sprint 3.xlsx
+++ b/Docs/Burndown/BurndownChart Sprint 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Luiz\Desktop\Fazenda-Urbana\Docs\Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E299726-39A3-455A-A132-92895E3377FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1714959-79C4-45B8-A0D0-5A56703B8676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BA74DF6-2A1D-4A46-8400-2B3B0F69CD68}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Atual</t>
   </si>
@@ -369,6 +369,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -381,10 +384,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -725,22 +725,22 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1915,7 +1915,7 @@
   <dimension ref="B1:S58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,26 +1934,26 @@
   <sheetData>
     <row r="1" spans="2:19" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:19" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="23"/>
     </row>
     <row r="3" spans="2:19" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1966,22 +1966,22 @@
       <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
     </row>
     <row r="5" spans="2:19" ht="57" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -1992,44 +1992,46 @@
         <f>IF(ISBLANK(C5),"Não Concluída","Concluída")</f>
         <v>Não Concluída</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
     </row>
     <row r="6" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="13"/>
+      <c r="C6" s="13" t="s">
+        <v>9</v>
+      </c>
       <c r="D6" s="17" t="str">
         <f>IF(ISBLANK(C6),"Não Concluída","Concluída")</f>
-        <v>Não Concluída</v>
-      </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
+        <v>Concluída</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
@@ -2040,20 +2042,20 @@
         <f>IF(ISBLANK(C7),"Não Concluída","Concluída")</f>
         <v>Não Concluída</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
     </row>
     <row r="8" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
@@ -2064,20 +2066,20 @@
         <f t="shared" ref="D8:D11" si="0">IF(ISBLANK(C8),"Não Concluída","Concluída")</f>
         <v>Não Concluída</v>
       </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
     </row>
     <row r="9" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
@@ -2088,87 +2090,91 @@
         <f t="shared" si="0"/>
         <v>Não Concluída</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
     </row>
     <row r="10" spans="2:19" ht="42.75" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="24"/>
+      <c r="C10" s="19" t="s">
+        <v>11</v>
+      </c>
       <c r="D10" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Não Concluída</v>
-      </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
+        <v>Concluída</v>
+      </c>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
     </row>
     <row r="11" spans="2:19" ht="42.75" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="14"/>
+      <c r="C11" s="24" t="s">
+        <v>12</v>
+      </c>
       <c r="D11" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Não Concluída</v>
-      </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
+        <v>Concluída</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
     </row>
     <row r="12" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="13"/>
       <c r="D12" s="17"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
     </row>
     <row r="13" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
@@ -2290,33 +2296,33 @@
       <c r="H22" s="1">
         <v>7</v>
       </c>
-      <c r="I22" s="23">
+      <c r="I22" s="1">
         <f>H22-COUNTIF($C$5:$C$11,I20)</f>
         <v>7</v>
       </c>
-      <c r="J22" s="23">
+      <c r="J22" s="1">
         <f t="shared" ref="J22:O22" si="1">I22-COUNTIF($C$5:$C$11,J20)</f>
-        <v>7</v>
-      </c>
-      <c r="K22" s="23">
+        <v>6</v>
+      </c>
+      <c r="K22" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="L22" s="23">
+        <v>6</v>
+      </c>
+      <c r="L22" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="M22" s="23">
+        <v>5</v>
+      </c>
+      <c r="M22" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="N22" s="23">
+        <v>4</v>
+      </c>
+      <c r="N22" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="O22" s="23">
+        <v>4</v>
+      </c>
+      <c r="O22" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2505,14 +2511,11 @@
     <mergeCell ref="B2:S2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C58 C12 C14 C16 C18 C20 C22 C24 C26 C28 C30 C32 C34 C36 C38 C40 C42 C44 C46 C48 C50 C52 C54 C56" xr:uid="{7916BFD7-4F52-48BB-AC13-B3A91C73A66F}">
       <formula1>$I$20:$K$20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C7 C11 C9 C8" xr:uid="{70B2616D-06B6-4BFE-ABE8-20F72E5AA62A}">
-      <formula1>$I$20:$O$20</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{F68F4EE4-6069-4FD0-9DAA-8C38F2DA31D0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C11" xr:uid="{70B2616D-06B6-4BFE-ABE8-20F72E5AA62A}">
       <formula1>$I$20:$O$20</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Atualizando a VI sprint
</commit_message>
<xml_diff>
--- a/Docs/Burndown/BurndownChart Sprint 3.xlsx
+++ b/Docs/Burndown/BurndownChart Sprint 3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Luiz\Desktop\Fazenda-Urbana\Docs\Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1714959-79C4-45B8-A0D0-5A56703B8676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4339D047-58F9-4713-9658-14AEC58F8CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BA74DF6-2A1D-4A46-8400-2B3B0F69CD68}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Atual</t>
   </si>
@@ -51,27 +51,6 @@
     <t>Gráfico</t>
   </si>
   <si>
-    <t>24/04/2024</t>
-  </si>
-  <si>
-    <t>25/04/2024</t>
-  </si>
-  <si>
-    <t>26/04/2024</t>
-  </si>
-  <si>
-    <t>27/04/2024</t>
-  </si>
-  <si>
-    <t>28/04/2024</t>
-  </si>
-  <si>
-    <t>29/04/2024</t>
-  </si>
-  <si>
-    <t>30/04/2024</t>
-  </si>
-  <si>
     <t>7)Gerar o script de criação de bancos e scripts de dados iniciais de testes (Roteiro de teste)</t>
   </si>
   <si>
@@ -87,17 +66,26 @@
     <t>2)Diagrama de implementação e Diagrama de sequência:</t>
   </si>
   <si>
-    <t>6)Elaborar o diagrama ER do banco de dados e o dicionário de dados:</t>
+    <t>1) Criar um cenário bem detalhado com regras do negócio, glossário do sistema, pesquisa de mercado, livros sobre o tema;</t>
   </si>
   <si>
-    <t>4) Definir e justificar o ciclo de vida de desenvolvimento de software:</t>
+    <t>8)Definir relatórios de gestão para análise de evolução dos negócios, análise de mercado, desempenho dos funcionários (RH)</t>
+  </si>
+  <si>
+    <t>13/05/2024</t>
+  </si>
+  <si>
+    <t>14/05/2024</t>
+  </si>
+  <si>
+    <t>15/05/2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +128,13 @@
     </font>
     <font>
       <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -372,6 +367,12 @@
     <xf numFmtId="14" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -382,9 +383,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -529,25 +527,25 @@
                   <c:v>Start</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24/04/2024</c:v>
+                  <c:v>9/5/2024</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25/04/2024</c:v>
+                  <c:v>10/5/2024</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26/04/2024</c:v>
+                  <c:v>11/5/2024</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27/04/2024</c:v>
+                  <c:v>12/5/2024</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28/04/2024</c:v>
+                  <c:v>13/05/2024</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29/04/2024</c:v>
+                  <c:v>14/05/2024</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30/04/2024</c:v>
+                  <c:v>15/05/2024</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -689,25 +687,25 @@
                   <c:v>Start</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24/04/2024</c:v>
+                  <c:v>9/5/2024</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25/04/2024</c:v>
+                  <c:v>10/5/2024</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>26/04/2024</c:v>
+                  <c:v>11/5/2024</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27/04/2024</c:v>
+                  <c:v>12/5/2024</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28/04/2024</c:v>
+                  <c:v>13/05/2024</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29/04/2024</c:v>
+                  <c:v>14/05/2024</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30/04/2024</c:v>
+                  <c:v>15/05/2024</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -725,22 +723,22 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1914,8 +1912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCAACB0F-709E-4DF4-B2CC-BA70FA833E4E}">
   <dimension ref="B1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,26 +1932,26 @@
   <sheetData>
     <row r="1" spans="2:19" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:19" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="25"/>
     </row>
     <row r="3" spans="2:19" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1966,215 +1964,209 @@
       <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-    </row>
-    <row r="5" spans="2:19" ht="57" x14ac:dyDescent="0.25">
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+    </row>
+    <row r="5" spans="2:19" ht="71.25" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="16" t="str">
         <f>IF(ISBLANK(C5),"Não Concluída","Concluída")</f>
         <v>Não Concluída</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-    </row>
-    <row r="6" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+    </row>
+    <row r="6" spans="2:19" ht="71.25" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>9</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C6" s="13"/>
       <c r="D6" s="17" t="str">
         <f>IF(ISBLANK(C6),"Não Concluída","Concluída")</f>
-        <v>Concluída</v>
-      </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="20"/>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+        <v>Não Concluída</v>
+      </c>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+      <c r="S6" s="22"/>
+    </row>
+    <row r="7" spans="2:19" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="16" t="str">
         <f>IF(ISBLANK(C7),"Não Concluída","Concluída")</f>
         <v>Não Concluída</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="20"/>
-    </row>
-    <row r="8" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+    </row>
+    <row r="8" spans="2:19" ht="57" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="16" t="str">
         <f t="shared" ref="D8:D11" si="0">IF(ISBLANK(C8),"Não Concluída","Concluída")</f>
         <v>Não Concluída</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-    </row>
-    <row r="9" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Não Concluída</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-    </row>
-    <row r="10" spans="2:19" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+    </row>
+    <row r="10" spans="2:19" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C10" s="19"/>
       <c r="D10" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Concluída</v>
-      </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-    </row>
-    <row r="11" spans="2:19" ht="42.75" x14ac:dyDescent="0.25">
+        <v>Não Concluída</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+    </row>
+    <row r="11" spans="2:19" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>12</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C11" s="20"/>
       <c r="D11" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Concluída</v>
-      </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
+        <v>Não Concluída</v>
+      </c>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
     </row>
     <row r="12" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="13"/>
       <c r="D12" s="17"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="20"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
     </row>
     <row r="13" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
@@ -2209,6 +2201,7 @@
       <c r="B16" s="4"/>
       <c r="C16" s="13"/>
       <c r="D16" s="17"/>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
@@ -2232,26 +2225,26 @@
       <c r="H20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I20" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>11</v>
+      <c r="I20" s="6">
+        <v>45540</v>
+      </c>
+      <c r="J20" s="6">
+        <v>45570</v>
+      </c>
+      <c r="K20" s="6">
+        <v>45601</v>
+      </c>
+      <c r="L20" s="6">
+        <v>45631</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2302,27 +2295,27 @@
       </c>
       <c r="J22" s="1">
         <f t="shared" ref="J22:O22" si="1">I22-COUNTIF($C$5:$C$11,J20)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K22" s="1">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M22" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="N22" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O22" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Requisitos funcionais e não funcionais
</commit_message>
<xml_diff>
--- a/Docs/Burndown/BurndownChart Sprint 3.xlsx
+++ b/Docs/Burndown/BurndownChart Sprint 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Luiz\Desktop\Fazenda-Urbana\Docs\Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4339D047-58F9-4713-9658-14AEC58F8CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0B093B-572E-4F3F-9FEF-0D91C475A54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BA74DF6-2A1D-4A46-8400-2B3B0F69CD68}"/>
   </bookViews>
@@ -726,19 +726,19 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1913,7 +1913,7 @@
   <dimension ref="B1:S58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,10 +2033,12 @@
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="12">
+        <v>45601</v>
+      </c>
       <c r="D7" s="16" t="str">
         <f>IF(ISBLANK(C7),"Não Concluída","Concluída")</f>
-        <v>Não Concluída</v>
+        <v>Concluída</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
@@ -2299,23 +2301,23 @@
       </c>
       <c r="K22" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M22" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N22" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O22" s="1">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>